<commit_message>
Create components class, add components examples
</commit_message>
<xml_diff>
--- a/Bills/test_file.xlsx
+++ b/Bills/test_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Documents\CEFET\2021_1\Energia solar\Atividades\Atividade 6\trabalho_solar\Bills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC24C54-2E0F-4A01-B99F-0C00A1B082D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7AFA9-C658-4A9D-BF0A-E2C32585601C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{7FC4A9E2-CA01-4E76-A93B-B738A45909A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7FC4A9E2-CA01-4E76-A93B-B738A45909A7}"/>
   </bookViews>
   <sheets>
     <sheet name="bill" sheetId="1" r:id="rId1"/>
@@ -37,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="30">
   <si>
     <t>month_year</t>
   </si>
@@ -128,9 +150,6 @@
   </si>
   <si>
     <t>x</t>
-  </si>
-  <si>
-    <t>equipmnet</t>
   </si>
 </sst>
 </file>
@@ -650,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CA8346-B121-4C4E-ADE4-BEE410D94DF9}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -1022,9 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64298701-20C0-488B-83DF-9DCE1CEDA862}">
   <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1032,8 +1049,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>25</v>
+      <c r="A1" t="str" cm="1">
+        <f t="array" ref="A1:A23">_xlfn._xlws.FILTER(ca_loads!A:A,ca_loads!A:A&lt;&gt;"","")</f>
+        <v>equipment</v>
       </c>
       <c r="B1" s="2">
         <v>0</v>
@@ -1109,8 +1127,8 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" t="str">
+        <v>notebook thiago empresa</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1146,8 +1164,8 @@
       <c r="Y2" s="1"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" t="str">
+        <v>notebook thiago pessoal</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1187,8 +1205,8 @@
       <c r="Y3" s="1"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
+      <c r="A4" t="str">
+        <v>notebook thaysa</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1224,8 +1242,8 @@
       <c r="Y4" s="1"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
+      <c r="A5" t="str">
+        <v>notebook jane</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1261,8 +1279,8 @@
       <c r="Y5" s="1"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
+      <c r="A6" t="str">
+        <v>geladeira</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
@@ -1338,8 +1356,8 @@
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
+      <c r="A7" t="str">
+        <v>microondas</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1369,8 +1387,8 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
+      <c r="A8" t="str">
+        <v>air frier</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1400,8 +1418,8 @@
       <c r="Y8" s="1"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
+      <c r="A9" t="str">
+        <v>televisao sala</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>29</v>
@@ -1433,8 +1451,8 @@
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
+      <c r="A10" t="str">
+        <v>televisao quarto</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1468,8 +1486,8 @@
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
+      <c r="A11" t="str">
+        <v>secador de cabelo</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1499,8 +1517,8 @@
       <c r="Y11" s="1"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
+      <c r="A12" t="str">
+        <v>maquina de lavar</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1530,8 +1548,8 @@
       <c r="Y12" s="1"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
+      <c r="A13" t="str">
+        <v>ventilador thiago</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -1573,8 +1591,8 @@
       <c r="Y13" s="1"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
+      <c r="A14" t="str">
+        <v>chuveiro jane</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1604,8 +1622,8 @@
       <c r="Y14" s="1"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
+      <c r="A15" t="str">
+        <v>chuveiro thiago</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1637,8 +1655,8 @@
       <c r="Y15" s="1"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
+      <c r="A16" t="str">
+        <v>celular thiago</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1668,8 +1686,8 @@
       <c r="Y16" s="1"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
+      <c r="A17" t="str">
+        <v>celular thaysa</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1699,8 +1717,8 @@
       <c r="Y17" s="1"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>19</v>
+      <c r="A18" t="str">
+        <v>celular jane</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1730,8 +1748,8 @@
       <c r="Y18" s="1"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
+      <c r="A19" t="str">
+        <v>computador thiago</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>29</v>
@@ -1767,8 +1785,8 @@
       <c r="Y19" s="1"/>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
+      <c r="A20" t="str">
+        <v>lampadas led</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>29</v>
@@ -1812,8 +1830,8 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>22</v>
+      <c r="A21" t="str">
+        <v>alexa</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>29</v>
@@ -1889,8 +1907,8 @@
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
+      <c r="A22" t="str">
+        <v>Filtro de agua</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>29</v>
@@ -1942,8 +1960,8 @@
       <c r="Y22" s="1"/>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>24</v>
+      <c r="A23" t="str">
+        <v>internet</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>29</v>
@@ -2028,14 +2046,18 @@
   <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
+      <c r="A1" s="1" t="str" cm="1">
+        <f t="array" ref="A1">_xlfn._xlws.FILTER(cc_loads!A:A,cc_loads!A:A&lt;&gt;"","")</f>
+        <v>equipment</v>
       </c>
       <c r="B1" s="2">
         <v>0</v>

</xml_diff>